<commit_message>
Making sure everything is working with the SharePoint doc
</commit_message>
<xml_diff>
--- a/data/sjp_data_catalog.xlsx
+++ b/data/sjp_data_catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre-my.sharepoint.com/personal/kcjoe_mitre_org/Documents/Documents/R/sjp-data-catalog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="6_{E8BFB680-39B2-7943-BA32-D6B47055C264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{151CC87A-CE9E-4D56-B7D7-78C4B32FCBBD}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="6_{E8BFB680-39B2-7943-BA32-D6B47055C264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D58985A-48FD-4213-8633-8EBC58512B12}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-975" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{5CA8705D-7F17-43E2-BAEE-43EEC2F1251D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5CA8705D-7F17-43E2-BAEE-43EEC2F1251D}"/>
   </bookViews>
   <sheets>
     <sheet name="guidelines" sheetId="15" r:id="rId1"/>
@@ -4483,8 +4483,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
@@ -4497,7 +4497,7 @@
     <col min="3" max="3" width="71.6640625" style="63" customWidth="1"/>
     <col min="4" max="5" width="28.6640625" style="69" customWidth="1"/>
     <col min="6" max="6" width="43.109375" style="64" customWidth="1"/>
-    <col min="7" max="7" width="20" style="18" customWidth="1"/>
+    <col min="7" max="7" width="34.44140625" style="18" customWidth="1"/>
     <col min="8" max="8" width="20.109375" style="64" customWidth="1"/>
     <col min="9" max="9" width="19" style="64" customWidth="1"/>
     <col min="10" max="10" width="30.44140625" style="69" customWidth="1"/>
@@ -9550,7 +9550,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -10158,9 +10158,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10367,27 +10370,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57084282-E38C-4E86-BAC4-63FB60E2432A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F90FE7-60B2-45D8-AA06-D09BDCE94429}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ada5df0c-07a0-4161-869c-31958091f7ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10412,9 +10403,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F90FE7-60B2-45D8-AA06-D09BDCE94429}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57084282-E38C-4E86-BAC4-63FB60E2432A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ada5df0c-07a0-4161-869c-31958091f7ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changing NAs in csv download to double dash
</commit_message>
<xml_diff>
--- a/data/sjp_data_catalog.xlsx
+++ b/data/sjp_data_catalog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre.sharepoint.com/sites/SocialJusticePlatformWSs/Shared Documents/Data Sources and Analysis/Data Catalog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre-my.sharepoint.com/personal/kcjoe_mitre_org/Documents/SJP Project/sjp-data-catalog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{286C9A01-D768-418D-95F5-CA792BDD9CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE48E6B0-8D28-4C4E-9169-894C77FCC61A}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{286C9A01-D768-418D-95F5-CA792BDD9CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB156317-27C9-4B71-B211-5F1935AD32EB}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-975" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{5CA8705D-7F17-43E2-BAEE-43EEC2F1251D}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="1252">
   <si>
     <t>Data Entry Guidelines</t>
   </si>
@@ -6287,10 +6287,10 @@
   <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -6416,9 +6416,7 @@
       <c r="F3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="69" t="s">
-        <v>406</v>
-      </c>
+      <c r="G3" s="69"/>
       <c r="H3" s="70" t="s">
         <v>23</v>
       </c>
@@ -7717,7 +7715,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="11" customFormat="1" ht="100.8">
+    <row r="34" spans="1:14" s="11" customFormat="1" ht="102">
       <c r="A34" s="37" t="s">
         <v>143</v>
       </c>
@@ -7906,9 +7904,7 @@
       <c r="F38" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="67" t="s">
-        <v>406</v>
-      </c>
+      <c r="G38" s="67"/>
       <c r="H38" s="68" t="s">
         <v>23</v>
       </c>
@@ -14118,6 +14114,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D114E827EF3DF44BA4E59A461CC4DA7" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43ca46e62ee0569e1c156693199bb51e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e" xmlns:ns3="ada5df0c-07a0-4161-869c-31958091f7ef" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3c2d7b02ff637bc90932a8cfde2bdc3" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e"/>
@@ -14339,27 +14355,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57084282-E38C-4E86-BAC4-63FB60E2432A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ada5df0c-07a0-4161-869c-31958091f7ef"/>
+    <ds:schemaRef ds:uri="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F90FE7-60B2-45D8-AA06-D09BDCE94429}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDD1FBAD-5FE3-4D6B-8D96-89B141478156}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14377,30 +14399,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F90FE7-60B2-45D8-AA06-D09BDCE94429}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57084282-E38C-4E86-BAC4-63FB60E2432A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ada5df0c-07a0-4161-869c-31958091f7ef"/>
-    <ds:schemaRef ds:uri="dd37c9a8-aab1-4b0a-adaf-d8ad8475de2e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>